<commit_message>
Added group list for Explore T2 and updated GDV4000 group list
</commit_message>
<xml_diff>
--- a/T2/GDV4000/GDV4000_25_26_Groups.xlsx
+++ b/T2/GDV4000/GDV4000_25_26_Groups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ian\TEACHING_25_26\2025_26\T2\GDV4000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98345A43-367B-4662-B541-DF1CB22A22CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA569E87-796C-4435-A38A-658FF6228620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="82440" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{587E5374-C9D8-4859-B380-F0EE43715D22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Team Member Name</t>
   </si>
@@ -203,7 +203,16 @@
     <t>Teen Spirit</t>
   </si>
   <si>
-    <t>Querying - Was in session 02/02/26</t>
+    <t>Noah Pearson</t>
+  </si>
+  <si>
+    <t>Max Hill</t>
+  </si>
+  <si>
+    <t>Rhys Stevens</t>
+  </si>
+  <si>
+    <t>Benji Fowler</t>
   </si>
 </sst>
 </file>
@@ -227,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -334,6 +349,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D9386D-6B8B-45BB-B130-317C6F7A19D9}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V69" sqref="V69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,61 +1058,96 @@
         <v>20305492</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="23"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="24">
+        <v>20325547</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="24">
+        <v>20326271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="24">
+        <v>20324344</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="24">
+        <v>20324307</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="24">
+        <v>20346682</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="15"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B56" s="15">
         <v>20300963</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B57" s="15">
         <v>20177773</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B58" s="15">
         <v>20265699</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B59" s="15">
         <v>20299200</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B60" s="15">
         <v>20299004</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="15">
-        <v>20325547</v>
-      </c>
-      <c r="C55" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>